<commit_message>
Updated successfully leave types validation for create , edit , updated , activate, deactivate and delete
</commit_message>
<xml_diff>
--- a/ExcelData/TC_LeaveBalance.xlsx
+++ b/ExcelData/TC_LeaveBalance.xlsx
@@ -37,10 +37,10 @@
     <t>leaveBalance</t>
   </si>
   <si>
-    <t xml:space="preserve">1 August 2023 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">31 August 2023 </t>
+    <t>2023-August-1</t>
+  </si>
+  <si>
+    <t>2023-August-31</t>
   </si>
 </sst>
 </file>
@@ -371,7 +371,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>